<commit_message>
Hid data excel sheet
</commit_message>
<xml_diff>
--- a/public/docs/Hurricanes-Report.xlsx
+++ b/public/docs/Hurricanes-Report.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\my-portfolio-cursor\my-portfolio-lovable\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03079190-40C7-4D01-8D8D-EA36C8D1EE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2858B04E-330E-4E5A-AAE9-1F635331CA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hurricane Map" sheetId="2" r:id="rId1"/>
-    <sheet name="Florida Hurricanes" sheetId="1" r:id="rId2"/>
+    <sheet name="Florida Hurricanes" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
@@ -426,7 +426,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -477,7 +477,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="↑ Double click media player icon&#10; above to open the 3D Map"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C63D4D6-40A3-1644-14E3-DDC0165156A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -513,7 +513,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Vlad" refreshedDate="46016.709295949076" createdVersion="8" refreshedVersion="8" recordCount="675" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Vlad" refreshedDate="46016.717308912041" createdVersion="8" refreshedVersion="8" recordCount="675" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>

</xml_diff>